<commit_message>
Test to verify error messages shown with duplicated travel documents (country/number) with in FAL5 and FAL6
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal5-Files/FAL 5-With-2same-NumberAndCountry.xlsx
+++ b/cypress/fixtures/Fal5-Files/FAL 5-With-2same-NumberAndCountry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal5-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSWTemp\nmsw-ui\cypress\fixtures\Fal5-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30D9BB8-1EC6-481E-BD38-46A339AF3024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460BA099-C807-4CB8-BE83-A948ED7C64FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAL 5" sheetId="1" r:id="rId1"/>
@@ -5037,9 +5037,6 @@
     <t>01/08/2029</t>
   </si>
   <si>
-    <t>Jane</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -5056,6 +5053,9 @@
   </si>
   <si>
     <t>10/01/1976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shamir   </t>
   </si>
 </sst>
 </file>
@@ -7237,27 +7237,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB976"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="19.81640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" style="6" customWidth="1"/>
+    <col min="1" max="2" width="19.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
-    <col min="6" max="8" width="19.81640625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="19.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" style="6" customWidth="1"/>
     <col min="10" max="10" width="22" style="6" customWidth="1"/>
-    <col min="11" max="11" width="25.6328125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="26.453125" style="6" customWidth="1"/>
-    <col min="13" max="26" width="8.81640625" style="6" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="14.453125" style="6" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" style="6" customWidth="1"/>
+    <col min="13" max="26" width="8.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" style="6" hidden="1" customWidth="1"/>
     <col min="28" max="16384" width="0" style="6" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="36" customFormat="1" ht="93">
+    <row r="1" spans="1:28" s="36" customFormat="1" ht="94.5">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -7369,7 +7369,7 @@
       <c r="Y3" s="45"/>
       <c r="Z3" s="46"/>
     </row>
-    <row r="4" spans="1:28" s="42" customFormat="1" ht="170.5">
+    <row r="4" spans="1:28" s="42" customFormat="1" ht="195">
       <c r="A4" s="37" t="s">
         <v>14</v>
       </c>
@@ -7421,7 +7421,7 @@
       <c r="Y4" s="40"/>
       <c r="Z4" s="41"/>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" ht="15">
       <c r="A5" s="56" t="s">
         <v>147</v>
       </c>
@@ -7473,7 +7473,7 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="15">
       <c r="A6" s="59" t="s">
         <v>1633</v>
       </c>
@@ -7511,7 +7511,7 @@
       <c r="M6" s="62"/>
       <c r="Z6" s="63"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" ht="15">
       <c r="A7" s="64" t="s">
         <v>1633</v>
       </c>
@@ -7529,13 +7529,13 @@
         <v>1640</v>
       </c>
       <c r="G7" s="66" t="s">
-        <v>1641</v>
+        <v>1651</v>
       </c>
       <c r="H7" s="66" t="s">
         <v>1642</v>
       </c>
       <c r="I7" s="60" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="J7" s="66" t="s">
         <v>1643</v>
@@ -7550,7 +7550,7 @@
       <c r="Z7" s="63"/>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" ht="15">
       <c r="A8" s="64" t="s">
         <v>1633</v>
       </c>
@@ -7562,10 +7562,10 @@
         <v>12345678</v>
       </c>
       <c r="E8" s="66" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="G8" s="66" t="s">
         <v>1641</v>
@@ -7574,7 +7574,7 @@
         <v>1642</v>
       </c>
       <c r="I8" s="60" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="J8" s="66" t="s">
         <v>1643</v>
@@ -7589,7 +7589,7 @@
       <c r="Z8" s="63"/>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" ht="15">
       <c r="A9" s="64" t="s">
         <v>1633</v>
       </c>
@@ -7603,17 +7603,17 @@
       <c r="E9" s="60" t="s">
         <v>1626</v>
       </c>
-      <c r="F9" s="60" t="s">
-        <v>1635</v>
+      <c r="F9" s="66" t="s">
+        <v>1646</v>
       </c>
       <c r="G9" s="66" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H9" s="66" t="s">
         <v>1645</v>
       </c>
-      <c r="H9" s="66" t="s">
-        <v>1646</v>
-      </c>
       <c r="I9" s="60" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="J9" s="66" t="s">
         <v>1643</v>
@@ -7628,7 +7628,7 @@
       <c r="Z9" s="63"/>
       <c r="AB9"/>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -7656,7 +7656,7 @@
       <c r="Y11" s="4"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -7684,7 +7684,7 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" ht="15">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -34698,15 +34698,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="50"/>
-    <col min="2" max="2" width="9.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="50"/>
+    <col min="2" max="2" width="9.42578125" style="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="58.5">
@@ -34714,7 +34714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.5">
+    <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="51" t="s">
         <v>26</v>
       </c>
@@ -34737,7 +34737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.5">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="50" t="s">
         <v>33</v>
       </c>
@@ -34760,7 +34760,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.5">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="50" t="s">
         <v>40</v>
       </c>
@@ -34783,7 +34783,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.5">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="50" t="s">
         <v>46</v>
       </c>
@@ -34806,7 +34806,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.5">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="50" t="s">
         <v>52</v>
       </c>
@@ -34829,7 +34829,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.5">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="50" t="s">
         <v>58</v>
       </c>
@@ -34852,7 +34852,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.5">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="50" t="s">
         <v>64</v>
       </c>
@@ -34875,7 +34875,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.5">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="50" t="s">
         <v>70</v>
       </c>
@@ -34898,7 +34898,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.5">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="50" t="s">
         <v>76</v>
       </c>
@@ -34921,7 +34921,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.5">
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="50" t="s">
         <v>83</v>
       </c>
@@ -34944,7 +34944,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.5">
+    <row r="12" spans="1:7" ht="15.75">
       <c r="A12" s="50" t="s">
         <v>90</v>
       </c>
@@ -34967,7 +34967,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.5">
+    <row r="13" spans="1:7" ht="15.75">
       <c r="A13" s="50" t="s">
         <v>96</v>
       </c>
@@ -34990,7 +34990,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.5">
+    <row r="14" spans="1:7" ht="15.75">
       <c r="A14" s="50" t="s">
         <v>102</v>
       </c>
@@ -35013,7 +35013,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.5">
+    <row r="15" spans="1:7" ht="15.75">
       <c r="A15" s="50" t="s">
         <v>108</v>
       </c>
@@ -35036,7 +35036,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.5">
+    <row r="16" spans="1:7" ht="15.75">
       <c r="A16" s="50" t="s">
         <v>115</v>
       </c>
@@ -35059,7 +35059,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.5">
+    <row r="17" spans="1:7" ht="15.75">
       <c r="A17" s="50" t="s">
         <v>121</v>
       </c>
@@ -35082,7 +35082,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.5">
+    <row r="18" spans="1:7" ht="15.75">
       <c r="A18" s="50" t="s">
         <v>127</v>
       </c>
@@ -35105,7 +35105,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.5">
+    <row r="19" spans="1:7" ht="15.75">
       <c r="A19" s="50" t="s">
         <v>133</v>
       </c>
@@ -35128,7 +35128,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.5">
+    <row r="20" spans="1:7" ht="15.75">
       <c r="A20" s="50" t="s">
         <v>139</v>
       </c>
@@ -35151,7 +35151,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.5">
+    <row r="21" spans="1:7" ht="15.75">
       <c r="A21" s="50" t="s">
         <v>146</v>
       </c>
@@ -35174,7 +35174,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.5">
+    <row r="22" spans="1:7" ht="15.75">
       <c r="A22" s="50" t="s">
         <v>153</v>
       </c>
@@ -35197,7 +35197,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.5">
+    <row r="23" spans="1:7" ht="15.75">
       <c r="A23" s="50" t="s">
         <v>159</v>
       </c>
@@ -35220,7 +35220,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.5">
+    <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="50" t="s">
         <v>165</v>
       </c>
@@ -35243,7 +35243,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.5">
+    <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="50" t="s">
         <v>171</v>
       </c>
@@ -35266,7 +35266,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.5">
+    <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="50" t="s">
         <v>177</v>
       </c>
@@ -35289,7 +35289,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.5">
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="50" t="s">
         <v>183</v>
       </c>
@@ -35312,7 +35312,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.5">
+    <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="50" t="s">
         <v>190</v>
       </c>
@@ -35335,7 +35335,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.5">
+    <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="50" t="s">
         <v>196</v>
       </c>
@@ -35358,7 +35358,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.5">
+    <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="50" t="s">
         <v>202</v>
       </c>
@@ -35381,7 +35381,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.5">
+    <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="50" t="s">
         <v>208</v>
       </c>
@@ -35404,7 +35404,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.5">
+    <row r="32" spans="1:7" ht="15.75">
       <c r="A32" s="50" t="s">
         <v>215</v>
       </c>
@@ -35427,7 +35427,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.5">
+    <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="50" t="s">
         <v>222</v>
       </c>
@@ -35450,7 +35450,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.5">
+    <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="50" t="s">
         <v>229</v>
       </c>
@@ -35473,7 +35473,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.5">
+    <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="50" t="s">
         <v>236</v>
       </c>
@@ -35496,7 +35496,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.5">
+    <row r="36" spans="1:7" ht="15.75">
       <c r="A36" s="50" t="s">
         <v>242</v>
       </c>
@@ -35519,7 +35519,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.5">
+    <row r="37" spans="1:7" ht="15.75">
       <c r="A37" s="50" t="s">
         <v>248</v>
       </c>
@@ -35542,7 +35542,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.5">
+    <row r="38" spans="1:7" ht="15.75">
       <c r="A38" s="50" t="s">
         <v>254</v>
       </c>
@@ -35565,7 +35565,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.5">
+    <row r="39" spans="1:7" ht="15.75">
       <c r="A39" s="50" t="s">
         <v>260</v>
       </c>
@@ -35588,7 +35588,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.5">
+    <row r="40" spans="1:7" ht="15.75">
       <c r="A40" s="50" t="s">
         <v>266</v>
       </c>
@@ -35611,7 +35611,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.5">
+    <row r="41" spans="1:7" ht="15.75">
       <c r="A41" s="50" t="s">
         <v>272</v>
       </c>
@@ -35634,7 +35634,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.5">
+    <row r="42" spans="1:7" ht="15.75">
       <c r="A42" s="50" t="s">
         <v>279</v>
       </c>
@@ -35657,7 +35657,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.5">
+    <row r="43" spans="1:7" ht="15.75">
       <c r="A43" s="50" t="s">
         <v>286</v>
       </c>
@@ -35680,7 +35680,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.5">
+    <row r="44" spans="1:7" ht="15.75">
       <c r="A44" s="50" t="s">
         <v>292</v>
       </c>
@@ -35703,7 +35703,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.5">
+    <row r="45" spans="1:7" ht="15.75">
       <c r="A45" s="50" t="s">
         <v>298</v>
       </c>
@@ -35726,7 +35726,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.5">
+    <row r="46" spans="1:7" ht="15.75">
       <c r="A46" s="50" t="s">
         <v>304</v>
       </c>
@@ -35749,7 +35749,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.5">
+    <row r="47" spans="1:7" ht="15.75">
       <c r="A47" s="50" t="s">
         <v>311</v>
       </c>
@@ -35772,7 +35772,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.5">
+    <row r="48" spans="1:7" ht="15.75">
       <c r="A48" s="50" t="s">
         <v>317</v>
       </c>
@@ -35795,7 +35795,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.5">
+    <row r="49" spans="1:7" ht="15.75">
       <c r="A49" s="50" t="s">
         <v>323</v>
       </c>
@@ -35818,7 +35818,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15.5">
+    <row r="50" spans="1:7" ht="15.75">
       <c r="A50" s="50" t="s">
         <v>329</v>
       </c>
@@ -35841,7 +35841,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15.5">
+    <row r="51" spans="1:7" ht="15.75">
       <c r="A51" s="50" t="s">
         <v>335</v>
       </c>
@@ -35864,7 +35864,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15.5">
+    <row r="52" spans="1:7" ht="15.75">
       <c r="A52" s="50" t="s">
         <v>342</v>
       </c>
@@ -35887,7 +35887,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.5">
+    <row r="53" spans="1:7" ht="15.75">
       <c r="A53" s="50" t="s">
         <v>349</v>
       </c>
@@ -35910,7 +35910,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.5">
+    <row r="54" spans="1:7" ht="15.75">
       <c r="A54" s="50" t="s">
         <v>355</v>
       </c>
@@ -35933,7 +35933,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.5">
+    <row r="55" spans="1:7" ht="15.75">
       <c r="A55" s="50" t="s">
         <v>361</v>
       </c>
@@ -35956,7 +35956,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15.5">
+    <row r="56" spans="1:7" ht="15.75">
       <c r="A56" s="50" t="s">
         <v>367</v>
       </c>
@@ -35979,7 +35979,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15.5">
+    <row r="57" spans="1:7" ht="15.75">
       <c r="A57" s="50" t="s">
         <v>373</v>
       </c>
@@ -36002,7 +36002,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15.5">
+    <row r="58" spans="1:7" ht="15.75">
       <c r="A58" s="50" t="s">
         <v>379</v>
       </c>
@@ -36025,7 +36025,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15.5">
+    <row r="59" spans="1:7" ht="15.75">
       <c r="A59" s="50" t="s">
         <v>386</v>
       </c>
@@ -36048,7 +36048,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.5">
+    <row r="60" spans="1:7" ht="15.75">
       <c r="A60" s="50" t="s">
         <v>392</v>
       </c>
@@ -36071,7 +36071,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15.5">
+    <row r="61" spans="1:7" ht="15.75">
       <c r="A61" s="50" t="s">
         <v>398</v>
       </c>
@@ -36094,7 +36094,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15.5">
+    <row r="62" spans="1:7" ht="15.75">
       <c r="A62" s="50" t="s">
         <v>404</v>
       </c>
@@ -36117,7 +36117,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15.5">
+    <row r="63" spans="1:7" ht="15.75">
       <c r="A63" s="50" t="s">
         <v>411</v>
       </c>
@@ -36140,7 +36140,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15.5">
+    <row r="64" spans="1:7" ht="15.75">
       <c r="A64" s="50" t="s">
         <v>418</v>
       </c>
@@ -36163,7 +36163,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15.5">
+    <row r="65" spans="1:7" ht="15.75">
       <c r="A65" s="50" t="s">
         <v>424</v>
       </c>
@@ -36186,7 +36186,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.5">
+    <row r="66" spans="1:7" ht="15.75">
       <c r="A66" s="50" t="s">
         <v>430</v>
       </c>
@@ -36209,7 +36209,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15.5">
+    <row r="67" spans="1:7" ht="15.75">
       <c r="A67" s="50" t="s">
         <v>436</v>
       </c>
@@ -36232,7 +36232,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15.5">
+    <row r="68" spans="1:7" ht="15.75">
       <c r="A68" s="50" t="s">
         <v>441</v>
       </c>
@@ -36255,7 +36255,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15.5">
+    <row r="69" spans="1:7" ht="15.75">
       <c r="A69" s="50" t="s">
         <v>446</v>
       </c>
@@ -36278,7 +36278,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15.5">
+    <row r="70" spans="1:7" ht="15.75">
       <c r="A70" s="50" t="s">
         <v>451</v>
       </c>
@@ -36301,7 +36301,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15.5">
+    <row r="71" spans="1:7" ht="15.75">
       <c r="A71" s="50" t="s">
         <v>456</v>
       </c>
@@ -36324,7 +36324,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.5">
+    <row r="72" spans="1:7" ht="15.75">
       <c r="A72" s="50" t="s">
         <v>462</v>
       </c>
@@ -36347,7 +36347,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.5">
+    <row r="73" spans="1:7" ht="15.75">
       <c r="A73" s="50" t="s">
         <v>468</v>
       </c>
@@ -36370,7 +36370,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15.5">
+    <row r="74" spans="1:7" ht="15.75">
       <c r="A74" s="50" t="s">
         <v>474</v>
       </c>
@@ -36393,7 +36393,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15.5">
+    <row r="75" spans="1:7" ht="15.75">
       <c r="A75" s="50" t="s">
         <v>480</v>
       </c>
@@ -36416,7 +36416,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15.5">
+    <row r="76" spans="1:7" ht="15.75">
       <c r="A76" s="50" t="s">
         <v>486</v>
       </c>
@@ -36439,7 +36439,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15.5">
+    <row r="77" spans="1:7" ht="15.75">
       <c r="A77" s="50" t="s">
         <v>492</v>
       </c>
@@ -36462,7 +36462,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15.5">
+    <row r="78" spans="1:7" ht="15.75">
       <c r="A78" s="50" t="s">
         <v>497</v>
       </c>
@@ -36485,7 +36485,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15.5">
+    <row r="79" spans="1:7" ht="15.75">
       <c r="A79" s="50" t="s">
         <v>502</v>
       </c>
@@ -36508,7 +36508,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15.5">
+    <row r="80" spans="1:7" ht="15.75">
       <c r="A80" s="50" t="s">
         <v>509</v>
       </c>
@@ -36531,7 +36531,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15.5">
+    <row r="81" spans="1:7" ht="15.75">
       <c r="A81" s="50" t="s">
         <v>516</v>
       </c>
@@ -36554,7 +36554,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15.5">
+    <row r="82" spans="1:7" ht="15.75">
       <c r="A82" s="50" t="s">
         <v>521</v>
       </c>
@@ -36577,7 +36577,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.5">
+    <row r="83" spans="1:7" ht="15.75">
       <c r="A83" s="50" t="s">
         <v>526</v>
       </c>
@@ -36600,7 +36600,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15.5">
+    <row r="84" spans="1:7" ht="15.75">
       <c r="A84" s="50" t="s">
         <v>531</v>
       </c>
@@ -36623,7 +36623,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.5">
+    <row r="85" spans="1:7" ht="15.75">
       <c r="A85" s="50" t="s">
         <v>536</v>
       </c>
@@ -36646,7 +36646,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15.5">
+    <row r="86" spans="1:7" ht="15.75">
       <c r="A86" s="50" t="s">
         <v>541</v>
       </c>
@@ -36669,7 +36669,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15.5">
+    <row r="87" spans="1:7" ht="15.75">
       <c r="A87" s="50" t="s">
         <v>546</v>
       </c>
@@ -36692,7 +36692,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.5">
+    <row r="88" spans="1:7" ht="15.75">
       <c r="A88" s="50" t="s">
         <v>551</v>
       </c>
@@ -36715,7 +36715,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15.5">
+    <row r="89" spans="1:7" ht="15.75">
       <c r="A89" s="50" t="s">
         <v>556</v>
       </c>
@@ -36738,7 +36738,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15.5">
+    <row r="90" spans="1:7" ht="15.75">
       <c r="A90" s="50" t="s">
         <v>561</v>
       </c>
@@ -36761,7 +36761,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15.5">
+    <row r="91" spans="1:7" ht="15.75">
       <c r="A91" s="50" t="s">
         <v>566</v>
       </c>
@@ -36784,7 +36784,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15.5">
+    <row r="92" spans="1:7" ht="15.75">
       <c r="A92" s="50" t="s">
         <v>573</v>
       </c>
@@ -36807,7 +36807,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15.5">
+    <row r="93" spans="1:7" ht="15.75">
       <c r="A93" s="50" t="s">
         <v>580</v>
       </c>
@@ -36830,7 +36830,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15.5">
+    <row r="94" spans="1:7" ht="15.75">
       <c r="A94" s="50" t="s">
         <v>586</v>
       </c>
@@ -36853,7 +36853,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15.5">
+    <row r="95" spans="1:7" ht="15.75">
       <c r="A95" s="50" t="s">
         <v>592</v>
       </c>
@@ -36876,7 +36876,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15.5">
+    <row r="96" spans="1:7" ht="15.75">
       <c r="A96" s="50" t="s">
         <v>597</v>
       </c>
@@ -36899,7 +36899,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15.5">
+    <row r="97" spans="1:7" ht="15.75">
       <c r="A97" s="50" t="s">
         <v>602</v>
       </c>
@@ -36922,7 +36922,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.5">
+    <row r="98" spans="1:7" ht="15.75">
       <c r="A98" s="50" t="s">
         <v>608</v>
       </c>
@@ -36945,7 +36945,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15.5">
+    <row r="99" spans="1:7" ht="15.75">
       <c r="A99" s="50" t="s">
         <v>615</v>
       </c>
@@ -36968,7 +36968,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15.5">
+    <row r="100" spans="1:7" ht="15.75">
       <c r="A100" s="50" t="s">
         <v>622</v>
       </c>
@@ -36991,7 +36991,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15.5">
+    <row r="101" spans="1:7" ht="15.75">
       <c r="A101" s="50" t="s">
         <v>628</v>
       </c>
@@ -37014,7 +37014,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15.5">
+    <row r="102" spans="1:7" ht="15.75">
       <c r="A102" s="50" t="s">
         <v>634</v>
       </c>
@@ -37037,7 +37037,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15.5">
+    <row r="103" spans="1:7" ht="15.75">
       <c r="A103" s="50" t="s">
         <v>641</v>
       </c>
@@ -37060,7 +37060,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15.5">
+    <row r="104" spans="1:7" ht="15.75">
       <c r="A104" s="50" t="s">
         <v>647</v>
       </c>
@@ -37083,7 +37083,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15.5">
+    <row r="105" spans="1:7" ht="15.75">
       <c r="A105" s="50" t="s">
         <v>653</v>
       </c>
@@ -37106,7 +37106,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15.5">
+    <row r="106" spans="1:7" ht="15.75">
       <c r="A106" s="50" t="s">
         <v>659</v>
       </c>
@@ -37129,7 +37129,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15.5">
+    <row r="107" spans="1:7" ht="15.75">
       <c r="A107" s="50" t="s">
         <v>664</v>
       </c>
@@ -37152,7 +37152,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15.5">
+    <row r="108" spans="1:7" ht="15.75">
       <c r="A108" s="50" t="s">
         <v>669</v>
       </c>
@@ -37175,7 +37175,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15.5">
+    <row r="109" spans="1:7" ht="15.75">
       <c r="A109" s="50" t="s">
         <v>674</v>
       </c>
@@ -37198,7 +37198,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15.5">
+    <row r="110" spans="1:7" ht="15.75">
       <c r="A110" s="50" t="s">
         <v>680</v>
       </c>
@@ -37221,7 +37221,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15.5">
+    <row r="111" spans="1:7" ht="15.75">
       <c r="A111" s="50" t="s">
         <v>685</v>
       </c>
@@ -37244,7 +37244,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15.5">
+    <row r="112" spans="1:7" ht="15.75">
       <c r="A112" s="50" t="s">
         <v>690</v>
       </c>
@@ -37267,7 +37267,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15.5">
+    <row r="113" spans="1:7" ht="15.75">
       <c r="A113" s="50" t="s">
         <v>697</v>
       </c>
@@ -37290,7 +37290,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15.5">
+    <row r="114" spans="1:7" ht="15.75">
       <c r="A114" s="50" t="s">
         <v>704</v>
       </c>
@@ -37313,7 +37313,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15.5">
+    <row r="115" spans="1:7" ht="15.75">
       <c r="A115" s="50" t="s">
         <v>711</v>
       </c>
@@ -37336,7 +37336,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15.5">
+    <row r="116" spans="1:7" ht="15.75">
       <c r="A116" s="50" t="s">
         <v>718</v>
       </c>
@@ -37359,7 +37359,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15.5">
+    <row r="117" spans="1:7" ht="15.75">
       <c r="A117" s="50" t="s">
         <v>724</v>
       </c>
@@ -37382,7 +37382,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15.5">
+    <row r="118" spans="1:7" ht="15.75">
       <c r="A118" s="50" t="s">
         <v>731</v>
       </c>
@@ -37405,7 +37405,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15.5">
+    <row r="119" spans="1:7" ht="15.75">
       <c r="A119" s="50" t="s">
         <v>737</v>
       </c>
@@ -37428,7 +37428,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15.5">
+    <row r="120" spans="1:7" ht="15.75">
       <c r="A120" s="50" t="s">
         <v>743</v>
       </c>
@@ -37451,7 +37451,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15.5">
+    <row r="121" spans="1:7" ht="15.75">
       <c r="A121" s="50" t="s">
         <v>749</v>
       </c>
@@ -37474,7 +37474,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15.5">
+    <row r="122" spans="1:7" ht="15.75">
       <c r="A122" s="50" t="s">
         <v>755</v>
       </c>
@@ -37497,7 +37497,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15.5">
+    <row r="123" spans="1:7" ht="15.75">
       <c r="A123" s="50" t="s">
         <v>760</v>
       </c>
@@ -37520,7 +37520,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15.5">
+    <row r="124" spans="1:7" ht="15.75">
       <c r="A124" s="50" t="s">
         <v>765</v>
       </c>
@@ -37543,7 +37543,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15.5">
+    <row r="125" spans="1:7" ht="15.75">
       <c r="A125" s="50" t="s">
         <v>770</v>
       </c>
@@ -37566,7 +37566,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15.5">
+    <row r="126" spans="1:7" ht="15.75">
       <c r="A126" s="50" t="s">
         <v>775</v>
       </c>
@@ -37589,7 +37589,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15.5">
+    <row r="127" spans="1:7" ht="15.75">
       <c r="A127" s="50" t="s">
         <v>781</v>
       </c>
@@ -37612,7 +37612,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15.5">
+    <row r="128" spans="1:7" ht="15.75">
       <c r="A128" s="50" t="s">
         <v>787</v>
       </c>
@@ -37635,7 +37635,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15.5">
+    <row r="129" spans="1:7" ht="15.75">
       <c r="A129" s="50" t="s">
         <v>793</v>
       </c>
@@ -37658,7 +37658,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15.5">
+    <row r="130" spans="1:7" ht="15.75">
       <c r="A130" s="50" t="s">
         <v>799</v>
       </c>
@@ -37681,7 +37681,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15.5">
+    <row r="131" spans="1:7" ht="15.75">
       <c r="A131" s="50" t="s">
         <v>805</v>
       </c>
@@ -37704,7 +37704,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15.5">
+    <row r="132" spans="1:7" ht="15.75">
       <c r="A132" s="50" t="s">
         <v>811</v>
       </c>
@@ -37727,7 +37727,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15.5">
+    <row r="133" spans="1:7" ht="15.75">
       <c r="A133" s="50" t="s">
         <v>816</v>
       </c>
@@ -37750,7 +37750,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="15.5">
+    <row r="134" spans="1:7" ht="15.75">
       <c r="A134" s="50" t="s">
         <v>822</v>
       </c>
@@ -37773,7 +37773,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15.5">
+    <row r="135" spans="1:7" ht="15.75">
       <c r="A135" s="50" t="s">
         <v>828</v>
       </c>
@@ -37796,7 +37796,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15.5">
+    <row r="136" spans="1:7" ht="15.75">
       <c r="A136" s="50" t="s">
         <v>833</v>
       </c>
@@ -37819,7 +37819,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15.5">
+    <row r="137" spans="1:7" ht="15.75">
       <c r="A137" s="50" t="s">
         <v>838</v>
       </c>
@@ -37842,7 +37842,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15.5">
+    <row r="138" spans="1:7" ht="15.75">
       <c r="A138" s="50" t="s">
         <v>843</v>
       </c>
@@ -37865,7 +37865,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15.5">
+    <row r="139" spans="1:7" ht="15.75">
       <c r="A139" s="50" t="s">
         <v>848</v>
       </c>
@@ -37888,7 +37888,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15.5">
+    <row r="140" spans="1:7" ht="15.75">
       <c r="A140" s="50" t="s">
         <v>854</v>
       </c>
@@ -37911,7 +37911,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15.5">
+    <row r="141" spans="1:7" ht="15.75">
       <c r="A141" s="50" t="s">
         <v>860</v>
       </c>
@@ -37934,7 +37934,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="15.5">
+    <row r="142" spans="1:7" ht="15.75">
       <c r="A142" s="50" t="s">
         <v>867</v>
       </c>
@@ -37957,7 +37957,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15.5">
+    <row r="143" spans="1:7" ht="15.75">
       <c r="A143" s="50" t="s">
         <v>874</v>
       </c>
@@ -37980,7 +37980,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15.5">
+    <row r="144" spans="1:7" ht="15.75">
       <c r="A144" s="50" t="s">
         <v>880</v>
       </c>
@@ -38003,7 +38003,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15.5">
+    <row r="145" spans="1:7" ht="15.75">
       <c r="A145" s="50" t="s">
         <v>886</v>
       </c>
@@ -38026,7 +38026,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="15.5">
+    <row r="146" spans="1:7" ht="15.75">
       <c r="A146" s="50" t="s">
         <v>892</v>
       </c>
@@ -38049,7 +38049,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15.5">
+    <row r="147" spans="1:7" ht="15.75">
       <c r="A147" s="50" t="s">
         <v>898</v>
       </c>
@@ -38072,7 +38072,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15.5">
+    <row r="148" spans="1:7" ht="15.75">
       <c r="A148" s="50" t="s">
         <v>905</v>
       </c>
@@ -38095,7 +38095,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15.5">
+    <row r="149" spans="1:7" ht="15.75">
       <c r="A149" s="50" t="s">
         <v>911</v>
       </c>
@@ -38118,7 +38118,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="15.5">
+    <row r="150" spans="1:7" ht="15.75">
       <c r="A150" s="50" t="s">
         <v>917</v>
       </c>
@@ -38141,7 +38141,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15.5">
+    <row r="151" spans="1:7" ht="15.75">
       <c r="A151" s="50" t="s">
         <v>923</v>
       </c>
@@ -38164,7 +38164,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15.5">
+    <row r="152" spans="1:7" ht="15.75">
       <c r="A152" s="50" t="s">
         <v>929</v>
       </c>
@@ -38187,7 +38187,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="15.5">
+    <row r="153" spans="1:7" ht="15.75">
       <c r="A153" s="50" t="s">
         <v>935</v>
       </c>
@@ -38210,7 +38210,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="15.5">
+    <row r="154" spans="1:7" ht="15.75">
       <c r="A154" s="50" t="s">
         <v>941</v>
       </c>
@@ -38233,7 +38233,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15.5">
+    <row r="155" spans="1:7" ht="15.75">
       <c r="A155" s="50" t="s">
         <v>946</v>
       </c>
@@ -38256,7 +38256,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="15.5">
+    <row r="156" spans="1:7" ht="15.75">
       <c r="A156" s="50" t="s">
         <v>952</v>
       </c>
@@ -38279,7 +38279,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="15.5">
+    <row r="157" spans="1:7" ht="15.75">
       <c r="A157" s="50" t="s">
         <v>958</v>
       </c>
@@ -38302,7 +38302,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="15.5">
+    <row r="158" spans="1:7" ht="15.75">
       <c r="A158" s="50" t="s">
         <v>963</v>
       </c>
@@ -38325,7 +38325,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="15.5">
+    <row r="159" spans="1:7" ht="15.75">
       <c r="A159" s="50" t="s">
         <v>968</v>
       </c>
@@ -38348,7 +38348,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15.5">
+    <row r="160" spans="1:7" ht="15.75">
       <c r="A160" s="50" t="s">
         <v>973</v>
       </c>
@@ -38371,7 +38371,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="15.5">
+    <row r="161" spans="1:7" ht="15.75">
       <c r="A161" s="50" t="s">
         <v>978</v>
       </c>
@@ -38394,7 +38394,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15.5">
+    <row r="162" spans="1:7" ht="15.75">
       <c r="A162" s="50" t="s">
         <v>984</v>
       </c>
@@ -38417,7 +38417,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="15.5">
+    <row r="163" spans="1:7" ht="15.75">
       <c r="A163" s="50" t="s">
         <v>990</v>
       </c>
@@ -38440,7 +38440,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="15.5">
+    <row r="164" spans="1:7" ht="15.75">
       <c r="A164" s="50" t="s">
         <v>996</v>
       </c>
@@ -38463,7 +38463,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15.5">
+    <row r="165" spans="1:7" ht="15.75">
       <c r="A165" s="50" t="s">
         <v>1002</v>
       </c>
@@ -38486,7 +38486,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15.5">
+    <row r="166" spans="1:7" ht="15.75">
       <c r="A166" s="50" t="s">
         <v>1007</v>
       </c>
@@ -38509,7 +38509,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15.5">
+    <row r="167" spans="1:7" ht="15.75">
       <c r="A167" s="50" t="s">
         <v>1012</v>
       </c>
@@ -38532,7 +38532,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15.5">
+    <row r="168" spans="1:7" ht="15.75">
       <c r="A168" s="50" t="s">
         <v>1018</v>
       </c>
@@ -38555,7 +38555,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="15.5">
+    <row r="169" spans="1:7" ht="15.75">
       <c r="A169" s="50" t="s">
         <v>1024</v>
       </c>
@@ -38578,7 +38578,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15.5">
+    <row r="170" spans="1:7" ht="15.75">
       <c r="A170" s="50" t="s">
         <v>1029</v>
       </c>
@@ -38601,7 +38601,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15.5">
+    <row r="171" spans="1:7" ht="15.75">
       <c r="A171" s="50" t="s">
         <v>1034</v>
       </c>
@@ -38624,7 +38624,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="15.5">
+    <row r="172" spans="1:7" ht="15.75">
       <c r="A172" s="50" t="s">
         <v>1039</v>
       </c>
@@ -38647,7 +38647,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="15.5">
+    <row r="173" spans="1:7" ht="15.75">
       <c r="A173" s="50" t="s">
         <v>1044</v>
       </c>
@@ -38670,7 +38670,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15.5">
+    <row r="174" spans="1:7" ht="15.75">
       <c r="A174" s="50" t="s">
         <v>1051</v>
       </c>
@@ -38693,7 +38693,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15.5">
+    <row r="175" spans="1:7" ht="15.75">
       <c r="A175" s="50" t="s">
         <v>1058</v>
       </c>
@@ -38716,7 +38716,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15.5">
+    <row r="176" spans="1:7" ht="15.75">
       <c r="A176" s="50" t="s">
         <v>1064</v>
       </c>
@@ -38739,7 +38739,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="15.5">
+    <row r="177" spans="1:7" ht="15.75">
       <c r="A177" s="50" t="s">
         <v>1070</v>
       </c>
@@ -38762,7 +38762,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="15.5">
+    <row r="178" spans="1:7" ht="15.75">
       <c r="A178" s="50" t="s">
         <v>1076</v>
       </c>
@@ -38785,7 +38785,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="15.5">
+    <row r="179" spans="1:7" ht="15.75">
       <c r="A179" s="50" t="s">
         <v>1083</v>
       </c>
@@ -38808,7 +38808,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="15.5">
+    <row r="180" spans="1:7" ht="15.75">
       <c r="A180" s="50" t="s">
         <v>1090</v>
       </c>
@@ -38831,7 +38831,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="15.5">
+    <row r="181" spans="1:7" ht="15.75">
       <c r="A181" s="50" t="s">
         <v>1096</v>
       </c>
@@ -38854,7 +38854,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="15.5">
+    <row r="182" spans="1:7" ht="15.75">
       <c r="A182" s="50" t="s">
         <v>1102</v>
       </c>
@@ -38877,7 +38877,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="15.5">
+    <row r="183" spans="1:7" ht="15.75">
       <c r="A183" s="50" t="s">
         <v>1107</v>
       </c>
@@ -39094,27 +39094,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="15.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.6" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="61" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" customWidth="1"/>
-    <col min="3" max="7" width="9.1796875"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="7" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.5">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" s="20" t="s">
         <v>1112</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="15">
       <c r="A2" s="21" t="s">
         <v>1113</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.5">
+    <row r="3" spans="1:1" ht="15">
       <c r="A3" s="22"/>
     </row>
-    <row r="4" spans="1:1" ht="170.5">
+    <row r="4" spans="1:1" ht="165.75">
       <c r="A4" s="23" t="s">
         <v>1114</v>
       </c>
@@ -39143,13 +39143,13 @@
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="15.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15.6" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="30" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" style="30" customWidth="1"/>
-    <col min="3" max="5" width="16.1796875" style="27" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="27"/>
-    <col min="8" max="16384" width="14.81640625" style="27"/>
+    <col min="1" max="1" width="16.140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="30" customWidth="1"/>
+    <col min="3" max="5" width="16.140625" style="27" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="27"/>
+    <col min="8" max="16384" width="14.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -39166,7 +39166,7 @@
       <c r="E1" s="79"/>
       <c r="F1" s="26"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="24" t="s">
         <v>1118</v>
       </c>
@@ -39178,7 +39178,7 @@
       <c r="E2" s="82"/>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="24" t="s">
         <v>1120</v>
       </c>
@@ -39269,7 +39269,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="24" t="s">
         <v>1141</v>
       </c>
@@ -39333,7 +39333,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="15">
       <c r="A21" s="24" t="s">
         <v>1157</v>
       </c>
@@ -41218,26 +41218,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -41474,10 +41454,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EF1FD61-C2E6-4843-9418-343E38DCD8AB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABE1220D-06A4-4F97-A70F-0D90EAC761EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -41494,20 +41505,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABE1220D-06A4-4F97-A70F-0D90EAC761EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EF1FD61-C2E6-4843-9418-343E38DCD8AB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>